<commit_message>
manualisasi data naive bayes
</commit_message>
<xml_diff>
--- a/Code/datasetsoriginal.xlsx
+++ b/Code/datasetsoriginal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radityarin/Documents/Kuliah/Text Mining/Tugas Akhir/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radityarin/Documents/Kuliah/Skripsi/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73814C97-C62B-D348-BB60-7E42DB3FA05E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614D3A64-26A4-2E4D-A006-16F2814DDE8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{E517DF0A-607D-7340-A759-990BF38B1593}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19840" xr2:uid="{E517DF0A-607D-7340-A759-990BF38B1593}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="43">
   <si>
     <t>mantap..sekali sy dr Jawa Timur ikut bangga Jakarta punya MRT. Indonesia maju</t>
   </si>
@@ -157,6 +151,9 @@
   </si>
   <si>
     <t>Hasil akhir</t>
+  </si>
+  <si>
+    <t>Netral</t>
   </si>
 </sst>
 </file>
@@ -517,14 +514,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26557E15-28C7-6D43-A4FE-B3046CD9969B}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="116" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
-    <col min="2" max="2" width="135.1640625" customWidth="1"/>
+    <col min="2" max="2" width="250.1640625" customWidth="1"/>
     <col min="3" max="3" width="10.5" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" hidden="1" customWidth="1"/>
@@ -570,32 +567,32 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="H2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J2" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -603,31 +600,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="H3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J3" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -635,63 +632,63 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="H4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J4" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
+      <c r="B5" t="s">
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J5" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -699,31 +696,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J6" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -731,63 +728,63 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J7" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
+      <c r="B8" t="s">
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="H8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J8" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -795,31 +792,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="H9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J9" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -827,63 +824,63 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="G10" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="H10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J10" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
+      <c r="B11" t="s">
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="G11" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="H11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J11" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -915,7 +912,7 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -947,7 +944,7 @@
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -979,7 +976,7 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1011,7 +1008,7 @@
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="L15" s="1"/>
     </row>
@@ -1044,7 +1041,7 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1076,7 +1073,7 @@
         <v>4</v>
       </c>
       <c r="J17" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1108,7 +1105,7 @@
         <v>4</v>
       </c>
       <c r="J18" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="L18" s="1"/>
     </row>
@@ -1141,7 +1138,7 @@
         <v>4</v>
       </c>
       <c r="J19" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1173,7 +1170,7 @@
         <v>4</v>
       </c>
       <c r="J20" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1205,39 +1202,39 @@
         <v>4</v>
       </c>
       <c r="J21" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
-        <v>24</v>
+      <c r="B22" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="G22" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I22">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -1245,31 +1242,31 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -1277,63 +1274,63 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="G24" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I24">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
-        <v>27</v>
+      <c r="B25" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="F25" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="G25" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I25">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -1341,31 +1338,31 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="G26" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I26">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -1373,63 +1370,63 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="G27" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I27">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
-        <v>30</v>
+      <c r="B28" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="G28" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I28">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J28" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -1437,31 +1434,31 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="G29" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I29">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J29" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
@@ -1469,63 +1466,63 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="G30" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I30">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J30" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
-        <v>33</v>
+      <c r="B31" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="G31" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I31">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>